<commit_message>
Tables created: employee, branch
Basic table created. Further edits will be done.

In branch table, mgr_id is a foreign key, that refers to emp_id in employee table.
</commit_message>
<xml_diff>
--- a/Database Schema.xlsx
+++ b/Database Schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="0" windowWidth="22104" windowHeight="9972" activeTab="1"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="22104" windowHeight="9972" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_Employee" sheetId="1" r:id="rId1"/>
@@ -318,9 +318,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -329,6 +326,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +916,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,7 +937,7 @@
       <c r="C1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="16" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1072,9 +1072,9 @@
       <c r="C11" s="6"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="17" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11"/>
-      <c r="D17" s="16"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -1130,13 +1130,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="8.88671875" style="13"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1147,7 +1147,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <v>500</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1158,7 +1158,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>501</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -1169,7 +1169,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>502</v>
       </c>
       <c r="B4" t="s">
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>503</v>
       </c>
       <c r="B5" t="s">
@@ -1191,7 +1191,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>504</v>
       </c>
       <c r="B6" t="s">
@@ -1202,7 +1202,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>505</v>
       </c>
       <c r="B7" t="s">
@@ -1213,7 +1213,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>506</v>
       </c>
       <c r="B8" t="s">
@@ -1279,7 +1279,7 @@
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1293,7 +1293,7 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>500</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1307,7 +1307,7 @@
       <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>501</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1321,7 +1321,7 @@
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>502</v>
       </c>
       <c r="C4" t="s">
@@ -1335,7 +1335,7 @@
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>503</v>
       </c>
       <c r="C5" t="s">
@@ -1349,7 +1349,7 @@
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>504</v>
       </c>
       <c r="C6" t="s">
@@ -1363,7 +1363,7 @@
       <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>505</v>
       </c>
       <c r="C7" t="s">
@@ -1377,7 +1377,7 @@
       <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>506</v>
       </c>
       <c r="C8" t="s">

</xml_diff>

<commit_message>
Some more functionalitites added
1. Display salary in descending order.
2. Calculate average salary of all employees.
3. Total amount bookshop has to pay its employees, i.e. total salary.
4. Find total quantity each branch sells.
</commit_message>
<xml_diff>
--- a/Database Schema.xlsx
+++ b/Database Schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="0" windowWidth="22104" windowHeight="9972" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="5616" yWindow="0" windowWidth="22104" windowHeight="9972" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_Employee" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1159,19 +1159,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="8" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1179,142 +1179,139 @@
         <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="13">
         <v>500</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="11">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="13">
         <v>501</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="11">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="13">
         <v>502</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
       <c r="B5" s="13">
         <v>503</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
       <c r="B6" s="13">
         <v>504</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>2</v>
       </c>
       <c r="B7" s="13">
         <v>505</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2</v>
       </c>
       <c r="B8" s="13">
         <v>506</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6">
+        <v>203</v>
+      </c>
+      <c r="D8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="6">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="9"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>